<commit_message>
added to beta testing excel sheet
</commit_message>
<xml_diff>
--- a/raresim_Beta Testing_Tracker.xlsx
+++ b/raresim_Beta Testing_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\raresim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CA1FA1-1EB3-46C2-B749-EF7165351045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279EA0C8-CA14-4756-9644-DC00EBB596CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="convert.py" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="90">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -88,9 +88,6 @@
     <t>Documentation</t>
   </si>
   <si>
-    <t>Are the help pages (ie. ?summix, ?ancestryData) clearly laid out with concise descriptions of parameters and data inputs along with simple and clear examples?</t>
-  </si>
-  <si>
     <t>Examples- Are the examples easy to follow; clear, concise, is the data used in the examples readily accessible for the user?</t>
   </si>
   <si>
@@ -106,45 +103,15 @@
     <t>Beta Testing</t>
   </si>
   <si>
-    <t>Reviewer Remarks (Include warning printed in R)</t>
-  </si>
-  <si>
     <t>Second Reviewer Response (if necessary)</t>
   </si>
   <si>
     <t>Code Functionality: Does code function as intended under all possible parameter designations?</t>
   </si>
   <si>
-    <t>Warnings and Errors</t>
-  </si>
-  <si>
-    <t>Objective fit warnings with scaled objective:</t>
-  </si>
-  <si>
-    <t>.5 &lt;= moderate fit &lt; 1.5</t>
-  </si>
-  <si>
-    <t>1.5 &lt;= poor fit</t>
-  </si>
-  <si>
-    <t>Objective fit warnings without scaled objective:</t>
-  </si>
-  <si>
-    <t>moderate fit</t>
-  </si>
-  <si>
-    <t>poor fit</t>
-  </si>
-  <si>
-    <t>#add other commentary about something going wrong or being unclear</t>
-  </si>
-  <si>
     <t>Reviewer Remarks (Include pull request #)</t>
   </si>
   <si>
-    <t>Suggested Warnings and Errors</t>
-  </si>
-  <si>
     <t>Reviewer response (drop down)</t>
   </si>
   <si>
@@ -164,12 +131,6 @@
       </rPr>
       <t xml:space="preserve"> convert.py</t>
     </r>
-  </si>
-  <si>
-    <t>Function: extract.py</t>
-  </si>
-  <si>
-    <t>Function: sim.py</t>
   </si>
   <si>
     <r>
@@ -223,42 +184,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Description: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Simulate new allele frequencies</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Parameters (with default values, if any):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
--h, --help                      show this help messgae and exit
--m SPARSE_MATRIX   Input sparse matrix path
--b EXP_BINS                Input expected bin sizes
--l INPUT_LEGEND       Input variant site legend
--L OUTPUT_LEGEND   Output variant site legend 
--H OUTPUT_HAP         Output compress hap file</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Parameters (with default values, if any): </t>
     </r>
     <r>
@@ -284,98 +209,13 @@
 -o Simulated_80k_9.controls.haps.gz.sm</t>
   </si>
   <si>
-    <t>Using a non .gz input file
--i /lib/raresim/test/data/Simulated_80k_9.controls.haps
- -o Simulated_80k_9.controls.haps.gz.sm</t>
-  </si>
-  <si>
-    <t>Omitting -i and -o parameters</t>
-  </si>
-  <si>
     <t>Not specifying .sm at the end of the output file
 -i /lib/raresim/test/data/Simulated_80k_9.controls.haps
  -o Simulated_80k_9.controls.haps.gz</t>
   </si>
   <si>
-    <t>Inputting a .sm file
--i
--o</t>
-  </si>
-  <si>
-    <t>Omitting -i parmater
--o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omitting -o parameter
--i </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inputting a non .hap file
--i
--o </t>
-  </si>
-  <si>
     <t xml:space="preserve">Example as given in the README
 -i lib/raresim/test/data/Simulated_80k_9.controls.haps
--o extracted_hap_subset.haps
--n 20
---seed 123 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omitting -i
--o extracted_hap_subset.haps
--n 20
---seed 123 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omitting -o
--i lib/raresim/test/data/Simulated_80k_9.controls.haps
--n 20
---seed 123 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omitting -n
--i lib/raresim/test/data/Simulated_80k_9.controls.haps
--o extracted_hap_subset.haps
---seed 123 </t>
-  </si>
-  <si>
-    <t>Omitting --seed
--i lib/raresim/test/data/Simulated_80k_9.controls.haps
--o extracted_hap_subset.haps
--n 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setting n as a non integer value
--i lib/raresim/test/data/Simulated_80k_9.controls.haps
--o extracted_hap_subset.haps
--n g
---seed 123 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setting n as a negative value
--i lib/raresim/test/data/Simulated_80k_9.controls.haps
--o extracted_hap_subset.haps
--n -10
---seed 123 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using -set SEED instead of --set SEED
--i lib/raresim/test/data/Simulated_80k_9.controls.haps
--o extracted_hap_subset.haps
--n 20
--seed 123 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inputting a .sm file instead of a .hap file
--i Simulated_80k_9.controls.haps.gz.sm
--o extracted_hap_subset.haps
--n 20
---seed 123 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inputting a .txt file
--i  lib/raresim/test/data/Expected_variants_functional.txt
 -o extracted_hap_subset.haps
 -n 20
 --seed 123 </t>
@@ -389,70 +229,802 @@
  -H new.hap.gz</t>
   </si>
   <si>
-    <t>Omitting -m
--b lib/raresim/test/data/Expected_variants_per_bin_80k.txt 
- -l lib/raresim/test/data/Simulated_80k.legend 
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Needs Work</t>
+  </si>
+  <si>
+    <t>I would specify somewhere in the README what a sparse matrix is</t>
+  </si>
+  <si>
+    <t>Reviewer Remarks (Include warning and or error message)</t>
+  </si>
+  <si>
+    <t>Using a non .gz input file
+-i /lib/raresim/test/data/Simulated_80k_9.controls.haps
+ -o Simulated_80k_9.controls.haps.sm</t>
+  </si>
+  <si>
+    <t>Inputting a .sm file
+-i Simulated_80k_9.controls.haps.gz.sm
+-o sm_input_Simulated_80k_9.controls.haps.gz.sm</t>
+  </si>
+  <si>
+    <t>Omitting -i parmater
+-o no_input_Simulated_80k_9.controls.haps.gz.sm \\
+OR
+-i
+-o no_input_Simulated_80k_9.controls.haps.gz.sm</t>
+  </si>
+  <si>
+    <t>Omitting -o parameter
+-i Simulated_80k_9.controls.haps.gz.sm \\
+OR
+-i Simulated_80k_9.controls.haps.gz.sm
+-o</t>
+  </si>
+  <si>
+    <t>Omitting -i and -o parameters
+-i
+-o
+OR
+convert.py</t>
+  </si>
+  <si>
+    <t>Throws: 
+convert.py: error: the following arguments are required: -o \\
+AND
+convert.py: error: argument -o: expected one argument \\
+respectively</t>
+  </si>
+  <si>
+    <t>Throws: 
+convert.py: error: the following arguments are required: -i \\
+AND
+convert.py: error: argument -i: expected one argument \\
+respectively</t>
+  </si>
+  <si>
+    <t>Throws: 
+convert.py: error: argument -i: expected one argument \\
+AND
+convert.py: error: the following arguments are required: -i, -o \\
+respectivley</t>
+  </si>
+  <si>
+    <t>Are the help pages (ie. -h, --help) clearly laid out with concise descriptions of parameters and data inputs along with simple and clear examples?</t>
+  </si>
+  <si>
+    <t>Are the help (ie. -h, --help) pages clearly laid out with concise descriptions of parameters and data inputs along with simple and clear examples?</t>
+  </si>
+  <si>
+    <t>the order of -n and --seed differ between the README and the actual help page, would fix just for consistency</t>
+  </si>
+  <si>
+    <t>There are no comments in the actual extract.py file; Could also include a brief description in the README example saying the example is doing</t>
+  </si>
+  <si>
+    <t>The convert.py file contains no comments;
+Could also add a brief description of what the example in the README is trying to accomplish</t>
+  </si>
+  <si>
+    <t>Reviewer Remarks (Include warning and errors)</t>
+  </si>
+  <si>
+    <t>Would note somewhere in the README that the output actually outputs 2 files, the .haps-sample file and the .haps-remainder file 
+Also provide a brief description of what the example is trying to accomplish</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If no input file path specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extract.py: error: argument -i: expected one argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If -i and no file path specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extract.py: error: the following arguments are required: -i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If no output file path specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extract.py: error: argument -o: expected one argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If -o and no file path specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extract.py: error: the following arguments are required: -o</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If n not specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extract.py: error: argument -n: expected one argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If -n and no number specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Traceback (most recent call last):
+  File "/home/math/siglersa/raresim/extract.py", line 52, in &lt;module&gt;
+    if __name__ == '__main__': main()
+  File "/home/math/siglersa/raresim/extract.py", line 39, in main
+    columnsToExtract = random.sample(range(0, size), args.num)
+  File "/usr/lib/python3.10/random.py", line 481, in sample
+    if not 0 &lt;= k &lt;= n:
+TypeError: '&lt;=' not supported between instances of 'int' and 'NoneType'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If no number after --seed specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extract.py: error: argument --seed: expected one argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If --seed and no number specified</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, runs</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Example as given, but omitting file path after -i or -i flag altogether       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example as given, but omitting file path after -o or -o flag altogether       </t>
+  </si>
+  <si>
+    <t>Example as given, but omitting number after -n or -n flag altogether</t>
+  </si>
+  <si>
+    <t>Example as given, but omitting number after --seed or --seed flag altogether</t>
+  </si>
+  <si>
+    <t>Example as given, but setting n as a non-integer value such as g</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If letter specified after -n, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extract.py: error: argument -n: invalid int value: 'g'
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Example as given, but specifying -n as a negative integer (e.g. -10) or a non integer value (e.g. 3.1415)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If negative number specified after -n, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Traceback (most recent call last):
+ ...
+ValueError: Sample larger than population or is negative
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If non-integer value specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+extract.py: error: argument -n: invalid int value: '3.1415'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Function: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>extract.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Function: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sim.py</t>
+    </r>
+  </si>
+  <si>
+    <t>The help page in python is longer than the help page in the README; I would update the README right after the Simulate new allele frequencies section to reflect what is displayed in python so it is consistent</t>
+  </si>
+  <si>
+    <t>Would include brief descritpions stating what the example is doing</t>
+  </si>
+  <si>
+    <t>No comments in the sim.py file</t>
+  </si>
+  <si>
+    <t>Reviewer Remarks (Include warning and error)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Outputs specified files, but also outputs new.legend-pruned-variants file. I would note this somewhere in the README, maybe give a discription of what this example is supposed to do.
+-I would add column names to the Input and New allele frequency distribution tables. First 2 columns are Lower and Upper MAC bin sizes, 3rd column is expected number of variants, and I think 4th is observed number of variants, but it is unclear.
+-The Input and New allele frequency distribution tables also output an extra row for any variants observed in any bin size greater than the highest MAC bin, but it only displays on value (the observed), so I would make a note of that in the README somewhere.
+-I also get slightly different outputs when I runt he example compared to what's in the README. Not sure if that's just do to randomness, but if it is I would note that somewhere. If it's not due to randomness, then that needs to be fixed.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example as given, but omitting file after -m or -m flag altogether
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If no file specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+sim.py: error: argument -m: expected one argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If file and -m flag also not specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+sim.py: error: the following arguments are required: -m</t>
+    </r>
+  </si>
+  <si>
+    <t>Example as given, but omitting file after -b or -b flag altogether</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If no file specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+sim.py: error: argument -b: expected one argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If file and -b flag also not specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If variants are split by functional/synonymous files must be provided for --functional_bins and --synonymous_bins</t>
+    </r>
+  </si>
+  <si>
+    <t>Example as given, but omitting file after -l or -l flag altogether</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If no file specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+sim.py: error: argument -l: expected one argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If file and -b flag also not specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Traceback (most recent call last):
+  File "/home/math/siglersa/raresim/sim.py", line 100, in &lt;module&gt;
+    if __name__ == '__main__': main()
+  File "/home/math/siglersa/raresim/sim.py", line 9, in main
+    legend_header, legend = read_legend(args.input_legend)
+  File "/home/math/siglersa/raresim/header.py", line 151, in read_legend
+    with open(legend_file_name) as f:
+TypeError: expected str, bytes or os.PathLike object, not NoneType</t>
+    </r>
+  </si>
+  <si>
+    <t>Example as given, but omitting file after -L or -L flag altogether</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If no file specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+sim.py: error: argument -L: expected one argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If file and -L flag also not specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Legend files not provided</t>
+    </r>
+  </si>
+  <si>
+    <t>Example as given, but omitting file after -H or -H flag altogether</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If no file specified, throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+sim.py: error: argument -H: expected one argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">If file and -H flag also not specified, throws:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sim.py: error: the following arguments are required: -H</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Example as give, but inputting a non-sparse matrix for -m flag e.g. -m Simulated_80k_9.controls.haps.gz
+</t>
+  </si>
+  <si>
+    <t>Throws:
+python3: alloc error in uint32_t_sparse_matrix_read().
+: Cannot allocate memory</t>
+  </si>
+  <si>
+    <r>
+      <t>Parameters (with default values, if any):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-h, --help                                                         show this help messgae and exit
+-m SPARSE_MATRIX                                    Input sparse matrix path
+-b EXP_BINS                                                   Input expected bin sizes
+--functional_bins EXP_FUN_BINS         Input expected bin sizes for functional variants
+--synonymous_bins EXP_SYN_BINS     Input expected bin sizes for synonymous variants
+-l INPUT_LEGEND                                         Input variant site legend
+-L OUTPUT_LEGEND                                    Output variant site legend 
+-H OUTPUT_HAP                                          Output compress hap file</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--f_only FUN_BINS_ONLY                         Input expected bin sizes for only functional variants
+--s_only SYN_BINS_ONLY                         Input expected bin sizes for only synonymous variants
+-z                                                                        Rows of zero are not removed
+-prob                                                                Rows are pruned allele by allele given a probability of removal
+--small_sample                                           Override error to allow for simulation of small sample size 
+--keep_protected                                      Rows in the legend marked with a 1 in the protected column will be accounted for but not pruned</t>
+    </r>
+  </si>
+  <si>
+    <t>Simulations that consider variant affect (functional/synonymous)</t>
+  </si>
+  <si>
+    <t>Example as given in the README
+-m chr19.block37.NFE.sim100.stratified.haps.gz.sm 
+ --functional_bins lib/raresim/test/data/Expected_variants_functional.txt 
+ --synonymous_bins lib/raresim/test/data/Expected_variants_synonymous.txt 
+ -l lib/raresim/test/data/chr19.block37.NFE.sim100.stratified.legend 
  -L new.legend 
  -H new.hap.gz</t>
   </si>
   <si>
-    <t>Omitting -b
--m Simulated_80k_9.controls.haps.gz.sm
- -l lib/raresim/test/data/Simulated_80k.legend 
- -L new.legend 
- -H new.hap.gz</t>
-  </si>
-  <si>
-    <t>Omitting -l
--m Simulated_80k_9.controls.haps.gz.sm
--b lib/raresim/test/data/Expected_variants_per_bin_80k.txt 
- -L new.legend 
- -H new.hap.gz</t>
-  </si>
-  <si>
-    <t>Omitting -L
--m Simulated_80k_9.controls.haps.gz.sm
--b lib/raresim/test/data/Expected_variants_per_bin_80k.txt 
- -l lib/raresim/test/data/Simulated_80k.legend 
- -H new.hap.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omitting -H
--m Simulated_80k_9.controls.haps.gz.sm
--b lib/raresim/test/data/Expected_variants_per_bin_80k.txt 
- -l lib/raresim/test/data/Simulated_80k.legend 
- -L new.legend </t>
-  </si>
-  <si>
-    <t>Inputting a non-sparse matrix
--m Simulated_80k_9.controls.haps.gz
--b lib/raresim/test/data/Expected_variants_per_bin_80k.txt 
- -l lib/raresim/test/data/Simulated_80k.legend 
- -L new.legend 
- -H new.hap.gz</t>
-  </si>
-  <si>
-    <t>Inputting a.legend file in place of bins
--m Simulated_80k_9.controls.haps.gz
--b lib/raresim/test/data/Simulated_80k.kegend
- -l lib/raresim/test/data/Simulated_80k.legend 
- -L new.legend 
- -H new.hap.gz</t>
-  </si>
-  <si>
-    <t>Inputting MAC bins in place of .legend
--m Simulated_80k_9.controls.haps.gz
--b lib/raresim/test/data/Expected_variants_per_bin_80k.txt 
- -l lib/raresim/test/data/Expected_variants_per_bin_80k.txt  
- -L new.legend 
- -H new.hap.gz</t>
+    <r>
+      <t>Descriptions: 
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Simulate new allele frequencies
+-Simulations that consider variant affect (functional/synonymous)
+     Simulations can independently be considered variants by their impact if 
+     1. the legend file (`-l` option) contains a column labeled fun where functional variants have the value fun, and synonymous variants have the value syn. 
+     2. separate expected bin size files are given for functional (`--functional_bins`) and synonymous (`--synonymous_bins`) variants
+-Prune only one type fo variant
+-Prune by given probabilities
+-Prune with protected variants
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">-Everything seems to output as it should
+-Again would add column names to AF distribution tables
+-I would give more detail as to whay sim.py actually does.     It says it simulates new AFs, but is it doing that by pruning certain variants? I'm assuming so because that’s the main goal of raresim, but I would just make it more explicit in the function description for sim.py.
+-Are the input AF distributions just the result of the pruning done without considering functional/synonymous status? It is unclear as to how those observed counts are being calculated for the input AF distributions . 
+-The new AF distribution tables differ from what’s in the README but I’m assuming that’s just due to randomness in the pruning. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +1035,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -524,7 +1103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -841,17 +1420,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BBB98C-CB6A-4A12-BCF2-53061E8E3915}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="155.5546875" customWidth="1"/>
     <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" customWidth="1"/>
+    <col min="3" max="3" width="57.88671875" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="24.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
@@ -860,17 +1439,17 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -912,26 +1491,41 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -940,38 +1534,56 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>17</v>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>4</v>
@@ -983,7 +1595,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -992,91 +1604,79 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>49</v>
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>53</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>31</v>
-      </c>
+      <c r="A33" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -1105,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4BF9AB-33CA-4B50-94E6-0DE74E28440B}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1121,17 +1721,17 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1142,7 +1742,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
@@ -1166,66 +1766,99 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>17</v>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>4</v>
@@ -1237,7 +1870,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -1246,63 +1879,97 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+    <row r="26" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+    <row r="27" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="240" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>63</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="A42" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -1331,15 +1998,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E63831-1160-4406-A302-FA13FD1BBDA7}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="142.88671875" customWidth="1"/>
     <col min="2" max="2" width="38.88671875" customWidth="1"/>
-    <col min="3" max="3" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="34.44140625" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
@@ -1347,18 +2014,18 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="219" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1366,16 +2033,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
@@ -1394,67 +2061,103 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>16</v>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>4</v>
@@ -1466,7 +2169,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -1475,52 +2178,100 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="172.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>72</v>
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1574,22 +2325,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
-    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1816,21 +2557,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
+    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
-    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1855,9 +2603,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
+    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added my simulation issues
</commit_message>
<xml_diff>
--- a/raresim_Beta Testing_Tracker.xlsx
+++ b/raresim_Beta Testing_Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\raresim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0E1A10-5EBD-4C8B-88F6-9E793EB8D0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71AD5D6-47C9-4FDF-B53F-B26019C2CFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="122">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1299,12 +1299,248 @@
     <t>-Same comments as --f_only above
 -I would also inlude a brief example in the README as well for the --s_only flag</t>
   </si>
+  <si>
+    <t>Bug Detected</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Throws</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 
+Traceback (most recent call last):
+  File "/home/math/siglersa/raresim/sim.py", line 100, in &lt;module&gt;
+    if __name__ == '__main__': main()
+  File "/home/math/siglersa/raresim/sim.py", line 69, in main
+    print_frequency_distribution(bins, bin_h, func_split, fun_only, syn_only)
+  File "/home/math/siglersa/raresim/header.py", line 304, in print_frequency_distribution
+    print_bin(bin_h['fun'], bins['fun'])
+  File "/home/math/siglersa/raresim/header.py", line 142, in print_bin
+    + str(len(bin_h[bin_id])))
+KeyError: 6</t>
+    </r>
+  </si>
+  <si>
+    <t>Additional Notes</t>
+  </si>
+  <si>
+    <t>-It doesn't work when the observed number of variants is less than the expected
+-It usually occurs for the [201, 400] bin where the expected number of functional variants is 0.43 for 100% and 0.36 for 80%, but the observed number of functional variants gets pruned down to 0 in the first step.</t>
+  </si>
+  <si>
+    <t>Same example as previous, but I combined the last two MAC bins for the 80% fun and 80% syn MAC bin estimates to try to avoid the error
+That is, instead of having 7 MAC bins where the last two were [21, 200] and [201, 400], I just have one [21, 400]. To get the expected number of variants (exp_var) for the MAC bin, I just added the exp_var of the [21, 200] and [201, 400] bins to get the exp_var for the [21, 400] bin. I did this for the functional and synonymous bins</t>
+  </si>
+  <si>
+    <t>Worked</t>
+  </si>
+  <si>
+    <t>My simulation scenario-Prune a hapgen haplotype file to 100% fun and 100% syn, then to 80% fun and 80% syn using RAREsim v2.1.1
+# Variables
+pop=NFE
+pruning=pruneSepRaresim
+nsim=20000
+pcase=100
+pconf=80
+int_prune=100
+ext_prune=80
+WD=/home/math/siglersa
+cd /storage/math/projects/RAREsim/Cases/Sim_20k/NFE/data
+for rep in $(eval echo "{$start..$end}")
+do
+# Prune fun and syn variants down to pcase %
+python3 ${WD}/raresim/sim.py \
+    -m chr19.block37.${pop}.sim${rep}.controls.haps.sm \
+    --functional_bins ${WD}/mastersProject/Input/MAC_bin_estimates_${nsim}_${pop}_fun_${pcase}.txt \
+    --synonymous_bins ${WD}/mastersProject/Input/MAC_bin_estimates_${nsim}_${pop}_syn_${pcase}.txt \
+    -l chr19.block37.${pop}.sim${rep}.copy.legend \
+    -L ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.${pcase}fun.${pcase}syn.legend \
+    -H ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.all.${pcase}fun.${pcase}syn.haps.gz
+# Convert -H hap file to sm
+python3 ${WD}/raresim/convert.py \
+    -i ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.all.${pcase}fun.${pcase}syn.haps.gz \
+    -o ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.all.${pcase}fun.${pcase}syn.haps.sm \
+# Prune fun and syn variants down again to pconf %
+python3 ${WD}/raresim/sim.py \
+    -m ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.all.${pcase}fun.${pcase}syn.haps.sm \
+    --functional_bins ${WD}/mastersProject/Input/MAC_bin_estimates_${nsim}_${pop}_fun_${pconf}.txt \
+    --synonymous_bins ${WD}/mastersProject/Input/MAC_bin_estimates_${nsim}_${pop}_syn_${pconf}.txt \
+    -l ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.${pcase}fun.${pcase}syn.legend \
+    -L ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.${pconf}fun.${pconf}syn.legend \
+    -H ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.all.${pconf}fun.${pconf}syn.haps.gz</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Traceback (most recent call last):
+  File "/home/math/siglersa/raresim/extract.py", line 52, in &lt;module&gt;
+    if __name__ == '__main__': main()
+  File "/home/math/siglersa/raresim/extract.py", line 36, in main
+    line = f.readline()
+  File "/usr/lib/python3.10/codecs.py", line 322, in decode
+    (result, consumed) = self._buffer_decode(data, self.errors, final)
+UnicodeDecodeError: 'utf-8' codec can't decode byte 0x8b in position 1: invalid start byte</t>
+    </r>
+  </si>
+  <si>
+    <t>-In the README example, the input file is a .hap file instead of a .hap.gz file as I'm using here. Not sure if that could be the issue
+-ALSO, I need to be able to subset the 80% pruned haplotype file with the same columns that are selected for the 100% pruned haplotype file (i.e., I need to make sure that the same columns that get extracted for cases in the 100% pruned file are the same columns that get extracted for the 80% pruned file). However, I'm not sure if setting the seed to the same number will extract the same columns between two different haplotype files</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Throws:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Traceback (most recent call last):
+  File "/home/math/siglersa/raresim/sim.py", line 100, in &lt;module&gt;
+    if __name__ == '__main__': main()
+  File "/home/math/siglersa/raresim/sim.py", line 90, in main
+    all_kept_rows = get_all_kept_rows(bin_h, R, func_split, fun_only, syn_only, args.z, args.keep_protected, legend)
+  File "/home/math/siglersa/raresim/header.py", line 338, in get_all_kept_rows
+    all_kept_rows = list(merge(all_kept_rows, sorted(R)))
+  File "/usr/lib/python3.10/heapq.py", line 353, in merge
+    _heapify(h)
+TypeError: '&lt;' not supported between instances of 'int' and 'str'</t>
+    </r>
+  </si>
+  <si>
+    <t>Using the same pipeline to prune the starting haplotype file to 100% fun and 100% syn and then to 80% fun and 80% syn using my work around for the MAC bins, I tried using the -z flag so that the outputted legend file for the 80% pruned step would hopefully be the same length as the outputted legened file from the 100% pruning step.
+The last step of the 3 step pipeline now looks like this:
+# Prune fun and syn variants down again to pconf %
+python3 ${WD}/raresim/sim.py \
+    -m ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.all.${pcase}fun.${pcase}syn.haps.sm \
+    --functional_bins ${WD}/mastersProject/Input/MAC_bin_estimates_${nsim}_${pop}_fun_${pconf}_6bins.txt \
+    --synonymous_bins ${WD}/mastersProject/Input/MAC_bin_estimates_${nsim}_${pop}_syn_${pconf}_6bins.txt \
+    -z \
+    -l ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.${pcase}fun.${pcase}syn.legend \
+    -L ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.${pconf}fun.${pconf}syn.legend \
+    -H ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.all.${pconf}fun.${pconf}syn.haps.gz</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example Warning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 
+WARNING: Lengths of legend 19029 and hap 19027 files do not match</t>
+    </r>
+  </si>
+  <si>
+    <t>When doing any of the pruning for my simulations, I noticed there were several warnings in the output file for some of the simulation replicates.
+For example, if I prune a starting haplotyoe file down to 80% fun and 80% syn variants usign the --functional_bins and --synonymous_bins flags, the warning appears for some of the simulation replicates. Same for if I prune down to 100% fun and 100% syn also using --functional_bins and --synonymous_bins flags, but it doesn't seem to pop the warning when I prune the 100% hap file down again to 80% fun and 80% syn (probably because it's using the hap and legend file from the 100% pruned step, which must match, to do the 80% pruned step).
+The warnings also appear if I use just the -b flag or the --f_only flag.</t>
+  </si>
+  <si>
+    <t>Using my simulation framework to subset the 100% fun and 100% syn pruned haplotype file to be able to create 3 datasets, none of which should have overlapping columns (aka individuals), but all have the same rows as the 100% pruned haplotype file
+# define parameters
+pop=NFE
+pruning=pruneSepRaresim
+pconf=100
+int_prune=100
+ext_prune=80
+Ncase=10000
+Nint=10000
+Ncc=20000
+end=100
+start=$(($end-99))
+WD=/home/math/siglersa
+### Start loop through 100 simulation replicates
+for rep in $(eval echo "{$start..$end}")
+do
+# Extract cases from pconf % pruned haplotype file
+python3 ${WD}/raresim/extract.py \
+    -i "${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/chr19.block37.${pop}.sim${rep}.all.${pconf}fun.${pconf}syn.haps.gz" \
+    -o "${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/datasets/chr19.block37.${pop}.sim${rep}.cases.${pconf}fun.${pconf}syn.haps.gz" \
+    -n ${Ncase} \
+    --seed 13
+# Extract internal controls from pconf % pruned haplotype REMAINDER file
+python3 ${WD}/raresim/extract.py \
+    -i ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/datasets/chr19.block37.${pop}.sim${rep}.cases.${pconf}fun.${pconf}syn.haps.gz-remainder \
+    -o ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/datasets/chr19.block37.${pop}.sim${rep}.internal.controls.${pconf}fun.${pconf}syn.haps.gz \
+    -n ${Nint} \
+    --seed 13
+# Extract external controls from internal controls REMAINDER file-should be all that's leftover
+python3 ${WD}/raresim/extract.py \
+    -i ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/datasets/chr19.block37.${pop}.sim${rep}.internal.controls.${pconf}fun.${pconf}syn.haps.gz-remainder \
+    -o ${WD}/mastersProject/20K_${pop}/${pruning}/${int_prune}v${ext_prune}/datasets/chr19.block37.${pop}.sim${rep}.common.controls.${pconf}fun.${pconf}syn.haps.gz \
+    -n ${Ncc} \
+    --seed 13
+done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-These are all done using Megan's haplotype files on the server under /storage/math/projects/RAREsim/Cases/Sim_20k/NFE/data
+-Not sure if some of the variants are getting cut off when the .haps.gz file got converted to the .haps.sm format </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1334,8 +1570,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1354,6 +1597,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD1D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1367,7 +1622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1393,12 +1648,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFD1D1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1709,7 +1994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BBB98C-CB6A-4A12-BCF2-53061E8E3915}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -1992,8 +2277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4BF9AB-33CA-4B50-94E6-0DE74E28440B}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2001,7 +2286,7 @@
     <col min="1" max="1" width="140.6640625" customWidth="1"/>
     <col min="2" max="2" width="35.109375" customWidth="1"/>
     <col min="3" max="3" width="45.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="24.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
@@ -2148,7 +2433,7 @@
         <v>52</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>5</v>
@@ -2246,8 +2531,19 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
+    <row r="31" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
@@ -2283,10 +2579,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E63831-1160-4406-A302-FA13FD1BBDA7}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2294,7 +2590,7 @@
     <col min="1" max="1" width="142.88671875" customWidth="1"/>
     <col min="2" max="2" width="38.88671875" customWidth="1"/>
     <col min="3" max="3" width="50.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="5" width="34.44140625" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
@@ -2447,7 +2743,7 @@
         <v>71</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>5</v>
@@ -2473,14 +2769,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:11" s="17" customFormat="1" ht="273" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="18" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2555,18 +2851,18 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:4" s="17" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="18" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>90</v>
       </c>
@@ -2577,7 +2873,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>91</v>
       </c>
@@ -2588,7 +2884,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>93</v>
       </c>
@@ -2599,7 +2895,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>77</v>
       </c>
@@ -2610,7 +2906,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="207.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="207.6" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>97</v>
       </c>
@@ -2621,7 +2917,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>78</v>
       </c>
@@ -2632,7 +2928,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>80</v>
       </c>
@@ -2643,7 +2939,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="286.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>99</v>
       </c>
@@ -2654,30 +2950,79 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
+    <row r="42" spans="1:4" s="12" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="10"/>
+    </row>
+    <row r="44" spans="1:4" s="12" customFormat="1" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" s="13"/>
+    </row>
+    <row r="45" spans="1:4" s="12" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+    <row r="47" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B47" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
+    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B48" t="s">
         <v>104</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added pruned-variant legend file issue
</commit_message>
<xml_diff>
--- a/raresim_Beta Testing_Tracker.xlsx
+++ b/raresim_Beta Testing_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\raresim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71AD5D6-47C9-4FDF-B53F-B26019C2CFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295FCB35-94D8-4185-9AE2-C8AC069ADEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="125">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1534,6 +1534,15 @@
   <si>
     <t xml:space="preserve">-These are all done using Megan's haplotype files on the server under /storage/math/projects/RAREsim/Cases/Sim_20k/NFE/data
 -Not sure if some of the variants are getting cut off when the .haps.gz file got converted to the .haps.sm format </t>
+  </si>
+  <si>
+    <t>For example, in sim replicate 3, the 100% pruned legend file contains 1364 variants and the 80% pruned legend file contains 1107 variants, so the 80% pruned-variants legend file should contain 257 variants (since that's the difference between 1364 and 1107), but it only contains 256 variants, so it's off by one variant.</t>
+  </si>
+  <si>
+    <t>-Not sure if this could be an issue in converting the 100% .haps.gz file into a .haps.sm file or the pruned-variants file isn't capturing all of the variants that get pruned</t>
+  </si>
+  <si>
+    <t>When using RAREsim v2.1.1 to prune a starting haplotype file to 100% fun and syn and then to 80% fun and syn variants as detailed in 4 cells above, there is a discrepancy between the legend and pruned-variant legend files</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1655,12 +1664,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2532,7 +2535,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="17" t="s">
         <v>120</v>
       </c>
       <c r="B31" s="12" t="s">
@@ -2579,10 +2582,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E63831-1160-4406-A302-FA13FD1BBDA7}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2769,14 +2772,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="17" customFormat="1" ht="273" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:11" s="15" customFormat="1" ht="273" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="16" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2851,14 +2854,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="17" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+    <row r="33" spans="1:4" s="15" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="16" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2965,7 +2968,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" s="9" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B43" s="9" t="s">
@@ -2974,10 +2977,10 @@
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" s="12" customFormat="1" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="12" t="s">
         <v>107</v>
       </c>
       <c r="C44" s="12" t="s">
@@ -2986,10 +2989,10 @@
       <c r="D44" s="13"/>
     </row>
     <row r="45" spans="1:4" s="12" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="12" t="s">
         <v>107</v>
       </c>
       <c r="C45" s="12" t="s">
@@ -2999,30 +3002,44 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:4" s="12" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
+    <row r="48" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="B47" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="B48" t="s">
         <v>104</v>
       </c>
       <c r="C48" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3077,22 +3094,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
-    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3319,21 +3326,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
+    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
-    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3358,9 +3372,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
+    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added issue with .legend-pruned-variants
</commit_message>
<xml_diff>
--- a/raresim_Beta Testing_Tracker.xlsx
+++ b/raresim_Beta Testing_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\raresim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295FCB35-94D8-4185-9AE2-C8AC069ADEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02758A51-D905-44E1-8295-21E03E9EE98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CBC82E3D-763F-40EC-B435-B43D17F2C6D6}"/>
   </bookViews>
@@ -3094,12 +3094,22 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
+    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3326,28 +3336,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="44ad9495-3741-4708-b440-876241155999" xsi:nil="true"/>
-    <SharedWithUsers xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44ad9495-3741-4708-b440-876241155999">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
+    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3372,12 +3375,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D535DE9-7631-4DA5-81A4-781256D545AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD35D980-7D34-404D-8A66-AF4A38B0629C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="44ad9495-3741-4708-b440-876241155999"/>
-    <ds:schemaRef ds:uri="98305de1-6b4d-4e48-ba1d-6a2d8f079fc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>